<commit_message>
replaced regional valuebox functions with a general valuebox function that works for both national and regional data
</commit_message>
<xml_diff>
--- a/data/cleaning_rules_contacts.xlsx
+++ b/data/cleaning_rules_contacts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfe78da84aa7621c/WHO/GoContactR/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{F5CFE34E-85D1-440C-8767-9B4B4EA134F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4F921187-F36D-2C45-8158-FAC407BEB56B}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{F5CFE34E-85D1-440C-8767-9B4B4EA134F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CDC8D3D3-6AE4-FA41-BC08-74E083D1CA77}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{790F353E-F9E7-4D7A-B387-FF662969880B}"/>
+    <workbookView xWindow="-20120" yWindow="760" windowWidth="23260" windowHeight="12580" xr2:uid="{790F353E-F9E7-4D7A-B387-FF662969880B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="68">
   <si>
     <t>bad_spelling</t>
   </si>
@@ -153,43 +153,7 @@
     <t>prefecture</t>
   </si>
   <si>
-    <t>COYAH</t>
-  </si>
-  <si>
-    <t>Coyah</t>
-  </si>
-  <si>
-    <t>DIXINN</t>
-  </si>
-  <si>
-    <t>Dixin</t>
-  </si>
-  <si>
-    <t>DUBREKA</t>
-  </si>
-  <si>
-    <t>Dureka</t>
-  </si>
-  <si>
-    <t>N'ZEREKORE</t>
-  </si>
-  <si>
-    <t>Nzerekore</t>
-  </si>
-  <si>
-    <t>RATOMA</t>
-  </si>
-  <si>
-    <t>Ratoma</t>
-  </si>
-  <si>
     <t>Non specifie</t>
-  </si>
-  <si>
-    <t>LOLA</t>
-  </si>
-  <si>
-    <t>Lola</t>
   </si>
   <si>
     <t>lien_avec_le_cas</t>
@@ -710,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E1CE11A-6CA9-4E4C-8BF7-B1C6D545AACB}">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -735,7 +699,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -757,7 +721,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -771,7 +735,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -782,7 +746,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -793,7 +757,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -804,7 +768,7 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -815,7 +779,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -826,7 +790,7 @@
         <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -837,7 +801,7 @@
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -859,7 +823,7 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -881,7 +845,7 @@
         <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
         <v>25</v>
@@ -892,7 +856,7 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
         <v>25</v>
@@ -903,7 +867,7 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
         <v>25</v>
@@ -914,7 +878,7 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
         <v>25</v>
@@ -1120,10 +1084,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" t="s">
         <v>37</v>
-      </c>
-      <c r="B37" t="s">
-        <v>38</v>
       </c>
       <c r="C37" t="s">
         <v>36</v>
@@ -1134,340 +1098,274 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C39" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C40" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="B42" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C42" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C43" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C44" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>52</v>
+        <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C45" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="B46" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C46" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C47" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C48" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C49" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B50" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C50" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="B51" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="C51" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C52" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="B53" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C53" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="B54" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C54" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B56" t="s">
-        <v>66</v>
+        <v>13</v>
       </c>
       <c r="C56" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="B57" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="C57" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="B58" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C58" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B59" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C59" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C60" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B61" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C61" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="B62" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C62" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
-        <v>12</v>
-      </c>
-      <c r="B63" t="s">
-        <v>67</v>
-      </c>
-      <c r="C63" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>62</v>
-      </c>
-      <c r="B64" t="s">
-        <v>66</v>
-      </c>
-      <c r="C64" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>63</v>
-      </c>
-      <c r="B65" t="s">
-        <v>66</v>
-      </c>
-      <c r="C65" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>64</v>
-      </c>
-      <c r="B66" t="s">
-        <v>66</v>
-      </c>
-      <c r="C66" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>65</v>
-      </c>
-      <c r="B67" t="s">
-        <v>66</v>
-      </c>
-      <c r="C67" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>5</v>
-      </c>
-      <c r="B68" t="s">
-        <v>47</v>
-      </c>
-      <c r="C68" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
progress with reporting module
</commit_message>
<xml_diff>
--- a/data/cleaning_rules_contacts.xlsx
+++ b/data/cleaning_rules_contacts.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfe78da84aa7621c/WHO/GoContactR/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfe78da84aa7621c/WHO/GoContactR_CIV/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{F5CFE34E-85D1-440C-8767-9B4B4EA134F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CDC8D3D3-6AE4-FA41-BC08-74E083D1CA77}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="13_ncr:1_{F5CFE34E-85D1-440C-8767-9B4B4EA134F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{53ACDF50-BCBB-0F45-8983-A809F08E8CE7}"/>
   <bookViews>
-    <workbookView xWindow="-20120" yWindow="760" windowWidth="23260" windowHeight="12580" xr2:uid="{790F353E-F9E7-4D7A-B387-FF662969880B}"/>
+    <workbookView xWindow="66260" yWindow="-5120" windowWidth="25960" windowHeight="18500" activeTab="2" xr2:uid="{790F353E-F9E7-4D7A-B387-FF662969880B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
     <definedName name="Vaccination">OFFSET([1]Dico!$K$1,1,0,COUNTIFS([1]Dico!$K:$K,"&lt;&gt;"&amp;"")-1)</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="83">
   <si>
     <t>bad_spelling</t>
   </si>
@@ -244,13 +245,58 @@
   </si>
   <si>
     <t>XX</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>18-Mar-98</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>FSW</t>
+  </si>
+  <si>
+    <t>WINDOWED</t>
+  </si>
+  <si>
+    <t>WIDOWED</t>
+  </si>
+  <si>
+    <t>MaritalStatus</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>variable_name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +314,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -311,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -319,6 +373,9 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E1CE11A-6CA9-4E4C-8BF7-B1C6D545AACB}">
   <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView zoomScale="235" workbookViewId="0">
+      <selection sqref="A1:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1399,4 +1456,135 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D445F6FE-BAD1-9A44-BB43-0B173F36303B}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="307" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A15" xr:uid="{EAD7F63C-510F-3343-B316-30D47CAA645A}">
+      <formula1>Vaccination</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="A3" twoDigitTextYear="1"/>
+    <ignoredError sqref="A4 A5:A7" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>